<commit_message>
.gitignore file is modified
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF69C4F-B563-46F3-A9AF-21CD3DC79140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495146C5-5974-4698-856D-7972A0069D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="login" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>tc_id</t>
   </si>
@@ -54,6 +54,48 @@
   </si>
   <si>
     <t>SI_004</t>
+  </si>
+  <si>
+    <t>urlBasePage</t>
+  </si>
+  <si>
+    <t>landing-page</t>
+  </si>
+  <si>
+    <t>continental.automation+sale@gmail.com</t>
+  </si>
+  <si>
+    <t>Sale_The_Man_1</t>
+  </si>
+  <si>
+    <t>_The_Man_1</t>
+  </si>
+  <si>
+    <t>sale@gmail.com</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>expectedText</t>
+  </si>
+  <si>
+    <t>testType</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>The username or password you entered is invalid</t>
+  </si>
+  <si>
+    <t>ALL MY LICENCES</t>
   </si>
 </sst>
 </file>
@@ -173,7 +215,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -188,6 +229,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,28 +556,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -548,92 +590,119 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="9"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="9"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check menu items and logout are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAC362E-F299-41F8-81FC-7B7D584D150E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B520E-A363-4E01-90AE-52912FF40502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="Licences" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$B$3</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>tc_id</t>
   </si>
@@ -108,6 +109,54 @@
   </si>
   <si>
     <t>Sign in</t>
+  </si>
+  <si>
+    <t>attributeType</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>SI_005</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>validationMessage</t>
+  </si>
+  <si>
+    <t>negativeI</t>
+  </si>
+  <si>
+    <t>negativeII</t>
+  </si>
+  <si>
+    <t>SI_006</t>
+  </si>
+  <si>
+    <t>menuItems1</t>
+  </si>
+  <si>
+    <t>menuItems0</t>
+  </si>
+  <si>
+    <t>menuItems2</t>
+  </si>
+  <si>
+    <t>LICENCE OVERVIEW</t>
+  </si>
+  <si>
+    <t>USER MANAGEMENT</t>
+  </si>
+  <si>
+    <t>CHECKLIST MANAGEMENT</t>
+  </si>
+  <si>
+    <t>loginText</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
   </si>
 </sst>
 </file>
@@ -167,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +230,16 @@
         </stop>
         <stop position="1">
           <color theme="9" tint="0.40000610370189521"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF00B0F0"/>
         </stop>
       </gradientFill>
     </fill>
@@ -221,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -246,6 +305,12 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -256,6 +321,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,35 +654,39 @@
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="1" customWidth="1"/>
+    <col min="9" max="11" width="20.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="37.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -628,18 +703,23 @@
         <v>14</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -649,47 +729,55 @@
       <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -699,43 +787,278 @@
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="37.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+    </row>
+    <row r="2" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test scenaros for Account setting are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B520E-A363-4E01-90AE-52912FF40502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E5B001-FAEE-4E2C-A1C0-3D66C47963FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>tc_id</t>
   </si>
@@ -157,6 +157,45 @@
   </si>
   <si>
     <t>LOGIN</t>
+  </si>
+  <si>
+    <t>successfullySavedText</t>
+  </si>
+  <si>
+    <t>Your information was successfully saved</t>
+  </si>
+  <si>
+    <t>randomType</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>notradnom</t>
+  </si>
+  <si>
+    <t>firstnameAS</t>
+  </si>
+  <si>
+    <t>lastnameAS</t>
+  </si>
+  <si>
+    <t>accountFirstEmptyMessage</t>
+  </si>
+  <si>
+    <t>accountLastEmptyMessage</t>
+  </si>
+  <si>
+    <t>Field is required</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>saveButtonDisabled</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -280,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -301,7 +340,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -646,7 +684,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,25 +704,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -898,10 +936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,114 +952,186 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="37.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="16" width="21" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-    </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+    </row>
+    <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1033,11 +1143,16 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1051,11 +1166,16 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="8"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
user management page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E5B001-FAEE-4E2C-A1C0-3D66C47963FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224967A-73A2-41C3-8DD9-ED366118C3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
account settings check for not radom user is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224967A-73A2-41C3-8DD9-ED366118C3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D7AEF7-2D1E-4731-96B8-863343831B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Licences" sheetId="2" r:id="rId2"/>
+    <sheet name="Header" sheetId="2" r:id="rId2"/>
+    <sheet name="UserManagement" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">login!$A$3:$B$3</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="59">
   <si>
     <t>tc_id</t>
   </si>
@@ -165,15 +166,6 @@
     <t>Your information was successfully saved</t>
   </si>
   <si>
-    <t>randomType</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>notradnom</t>
-  </si>
-  <si>
     <t>firstnameAS</t>
   </si>
   <si>
@@ -196,6 +188,33 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>sasa_notrandom</t>
+  </si>
+  <si>
+    <t>stjepanovic_notrandom</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>randomTypeYesNo</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>sasa_NOTrandom</t>
+  </si>
+  <si>
+    <t>stjepanovic_NOTrandom</t>
   </si>
 </sst>
 </file>
@@ -255,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +298,16 @@
         </stop>
         <stop position="1">
           <color rgb="FF00B0F0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFF0000"/>
         </stop>
       </gradientFill>
     </fill>
@@ -319,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -349,6 +378,12 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,6 +400,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,7 +725,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,25 +745,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -938,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,29 +999,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
     </row>
     <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1011,25 +1052,25 @@
         <v>38</v>
       </c>
       <c r="J3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>40</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>24</v>
@@ -1064,15 +1105,292 @@
         <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="Q5" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16" width="21" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+    </row>
+    <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="N4" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>41</v>
@@ -1098,37 +1416,37 @@
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
         <v>39</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="M5" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>41</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add/delete technicians method added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D7AEF7-2D1E-4731-96B8-863343831B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166AE626-00EB-45B9-B5C0-E2D057B0A3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="62">
   <si>
     <t>tc_id</t>
   </si>
@@ -193,12 +193,6 @@
     <t>user</t>
   </si>
   <si>
-    <t>sasa_notrandom</t>
-  </si>
-  <si>
-    <t>stjepanovic_notrandom</t>
-  </si>
-  <si>
     <t>not</t>
   </si>
   <si>
@@ -215,6 +209,21 @@
   </si>
   <si>
     <t>stjepanovic_NOTrandom</t>
+  </si>
+  <si>
+    <t>firstNameTechnician</t>
+  </si>
+  <si>
+    <t>lastNameTechnician</t>
+  </si>
+  <si>
+    <t>emailTechnician</t>
+  </si>
+  <si>
+    <t>numTechnicians</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -979,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1052,7 +1061,7 @@
         <v>38</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>42</v>
@@ -1105,7 +1114,7 @@
         <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
@@ -1152,7 +1161,7 @@
         <v>39</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -1201,13 +1210,13 @@
         <v>39</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>46</v>
@@ -1258,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,12 +1283,12 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16" width="21" style="1" customWidth="1"/>
-    <col min="17" max="17" width="24" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="18" width="21" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1299,12 +1308,14 @@
       <c r="O1" s="22"/>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
-    </row>
-    <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="1:19" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1331,31 +1342,37 @@
         <v>38</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="M3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="P3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="Q3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="R3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="S3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1382,25 +1399,29 @@
         <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="10"/>
+        <v>52</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="5" t="s">
+      <c r="R4" s="10"/>
+      <c r="S4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1425,31 +1446,29 @@
         <v>39</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="8" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="Q5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1468,9 +1487,11 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1489,11 +1510,13 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="8"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
method for deleting technicians are expanded
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166AE626-00EB-45B9-B5C0-E2D057B0A3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D60A5-23AA-46D8-AB9C-4BABDC7D9842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
   <si>
     <t>tc_id</t>
   </si>
@@ -224,6 +224,21 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>positiveMessage</t>
+  </si>
+  <si>
+    <t>successfully created.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>rowNumber</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1267,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,12 +1298,12 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="18" width="21" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="20" width="21" style="1" customWidth="1"/>
+    <col min="21" max="21" width="24" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1310,12 +1325,14 @@
       <c r="Q1" s="22"/>
       <c r="R1" s="22"/>
       <c r="S1" s="22"/>
-    </row>
-    <row r="2" spans="1:19" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+    </row>
+    <row r="2" spans="1:21" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1345,34 +1362,40 @@
         <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="N3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="O3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="R3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="S3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="T3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="U3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1402,26 +1425,32 @@
         <v>52</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="10"/>
+      <c r="U4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1448,50 +1477,88 @@
       <c r="J5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="S5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="8"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="10"/>
+      <c r="U6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1504,19 +1571,23 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="P7" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="8"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
User Management section,negative scenario
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D60A5-23AA-46D8-AB9C-4BABDC7D9842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3E9AB-4552-4FFB-A283-DD79515B178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="72">
   <si>
     <t>tc_id</t>
   </si>
@@ -239,6 +239,21 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>sasa_techn_1</t>
+  </si>
+  <si>
+    <t>sasa_techn_1@kik.com</t>
+  </si>
+  <si>
+    <t>userAlreadyExists</t>
+  </si>
+  <si>
+    <t>Username provided already exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Username provided already exists</t>
   </si>
 </sst>
 </file>
@@ -372,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -408,6 +423,7 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,25 +785,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1023,29 +1039,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
     </row>
     <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1282,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,33 +1320,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
     </row>
     <row r="2" spans="1:21" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1354,7 +1370,9 @@
       <c r="G3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="I3" s="14" t="s">
         <v>38</v>
       </c>
@@ -1558,32 +1576,131 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5" t="s">
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="8"/>
+      <c r="Q7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="10"/>
+      <c r="U7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="U8" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
licenceAllocated test is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3E9AB-4552-4FFB-A283-DD79515B178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17A9677-887A-422D-8CD4-7FE25F96CCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="75">
   <si>
     <t>tc_id</t>
   </si>
@@ -223,9 +223,6 @@
     <t>numTechnicians</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>positiveMessage</t>
   </si>
   <si>
@@ -254,6 +251,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Username provided already exists</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>invalidEmailMessage</t>
+  </si>
+  <si>
+    <t>E-mail must be valid</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -387,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -423,7 +432,6 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,25 +793,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1039,29 +1047,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
     </row>
     <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1298,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,41 +1322,42 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="20" width="21" style="1" customWidth="1"/>
-    <col min="21" max="21" width="24" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="21" width="21" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-    </row>
-    <row r="2" spans="1:21" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-    </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+    </row>
+    <row r="2" spans="1:22" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1380,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>38</v>
@@ -1380,7 +1389,7 @@
         <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>60</v>
@@ -1395,25 +1404,28 @@
         <v>59</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="S3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="T3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="U3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="V3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1443,32 +1455,33 @@
         <v>52</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="P4" s="10"/>
       <c r="Q4" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="R4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="S4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="10"/>
+      <c r="V4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1496,32 +1509,33 @@
         <v>51</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="P5" s="8"/>
       <c r="Q5" s="8" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1551,32 +1565,33 @@
         <v>52</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="S6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="10"/>
+      <c r="V6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>36</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>39</v>
@@ -1608,38 +1623,39 @@
         <v>51</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="P7" s="9"/>
       <c r="Q7" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="R7" s="10" t="s">
         <v>46</v>
       </c>
       <c r="S7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="10"/>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="10"/>
+      <c r="V7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1662,7 +1678,7 @@
         <v>36</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>39</v>
@@ -1671,40 +1687,109 @@
         <v>51</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="N8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="Q8" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="R8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="S8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T8" s="10"/>
-      <c r="U8" s="5" t="s">
+      <c r="U8" s="10"/>
+      <c r="V8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" s="10"/>
+      <c r="V9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
method for deleting users and than verification are splited
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17A9677-887A-422D-8CD4-7FE25F96CCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B38DD4-B3C6-4C25-A8E5-6A3135B5CDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="77">
   <si>
     <t>tc_id</t>
   </si>
@@ -263,6 +255,12 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>removeAllocationButtonText</t>
+  </si>
+  <si>
+    <t>REMOVE ALLOCATION</t>
   </si>
 </sst>
 </file>
@@ -416,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -435,25 +433,25 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,12 +1320,14 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="21" width="21" style="1" customWidth="1"/>
-    <col min="22" max="22" width="24" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="15" width="21" style="1" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" style="1" customWidth="1"/>
+    <col min="17" max="22" width="21" style="1" customWidth="1"/>
+    <col min="23" max="23" width="24" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1352,12 +1352,13 @@
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
-    </row>
-    <row r="2" spans="1:22" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1404,28 +1405,31 @@
         <v>59</v>
       </c>
       <c r="P3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="R3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="S3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="T3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="U3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="V3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1463,25 +1467,28 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10" t="s">
+      <c r="P4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="T4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="10"/>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="10"/>
+      <c r="W4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1516,26 +1523,27 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="S5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1574,24 +1582,25 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="S6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="T6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U6" s="10"/>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="10"/>
+      <c r="W6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1638,24 +1647,25 @@
         <v>67</v>
       </c>
       <c r="P7" s="9"/>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="S7" s="10" t="s">
         <v>46</v>
       </c>
       <c r="T7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="10"/>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="10"/>
+      <c r="W7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1701,27 +1711,28 @@
       <c r="O8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="R8" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="S8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="T8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U8" s="10"/>
-      <c r="V8" s="5" t="s">
+      <c r="V8" s="10"/>
+      <c r="W8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1767,29 +1778,30 @@
       <c r="O9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="S9" s="10" t="s">
         <v>46</v>
       </c>
       <c r="T9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="10"/>
+      <c r="W9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:W1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tests for search function through the usermanagement section
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B38DD4-B3C6-4C25-A8E5-6A3135B5CDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFEA23F-15D2-4DB6-A959-5D24851305AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="90">
   <si>
     <t>tc_id</t>
   </si>
@@ -233,9 +233,6 @@
     <t>sasa_techn_1</t>
   </si>
   <si>
-    <t>sasa_techn_1@kik.com</t>
-  </si>
-  <si>
     <t>userAlreadyExists</t>
   </si>
   <si>
@@ -261,6 +258,48 @@
   </si>
   <si>
     <t>REMOVE ALLOCATION</t>
+  </si>
+  <si>
+    <t>sasa_techn_servis</t>
+  </si>
+  <si>
+    <t>sasa_techn_platform</t>
+  </si>
+  <si>
+    <t>sasa_techn_system</t>
+  </si>
+  <si>
+    <t>SI_007</t>
+  </si>
+  <si>
+    <t>SI_008</t>
+  </si>
+  <si>
+    <t>sasa_techn_2</t>
+  </si>
+  <si>
+    <t>sasa_mail_1@kik.com</t>
+  </si>
+  <si>
+    <t>sasa_mail_2@kik.com</t>
+  </si>
+  <si>
+    <t>sasa_mail_3@kik.com</t>
+  </si>
+  <si>
+    <t>searchTechnician</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>searchedTechnician</t>
+  </si>
+  <si>
+    <t>emptySearch</t>
+  </si>
+  <si>
+    <t>doesnot_exist</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,14 +1359,15 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="15" width="21" style="1" customWidth="1"/>
-    <col min="16" max="16" width="27.42578125" style="1" customWidth="1"/>
-    <col min="17" max="22" width="21" style="1" customWidth="1"/>
-    <col min="23" max="23" width="24" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="17" width="21" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="27.42578125" style="1" customWidth="1"/>
+    <col min="20" max="25" width="21" style="1" customWidth="1"/>
+    <col min="26" max="26" width="24" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1353,12 +1393,15 @@
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
       <c r="W1" s="22"/>
-    </row>
-    <row r="2" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+    </row>
+    <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1424,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>38</v>
@@ -1405,31 +1448,40 @@
         <v>59</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="R3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="U3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="V3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="X3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="Y3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="Z3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1467,28 +1519,31 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="10" t="s">
-        <v>76</v>
-      </c>
+      <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
-      <c r="R4" s="10" t="s">
+      <c r="R4" s="10"/>
+      <c r="S4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V4" s="10"/>
-      <c r="W4" s="5" t="s">
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1524,26 +1579,29 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" s="10" t="s">
+      <c r="V5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="Y5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="Z5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1576,31 +1634,34 @@
         <v>63</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" s="10" t="s">
+      <c r="V6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V6" s="10"/>
-      <c r="W6" s="5" t="s">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +1684,7 @@
         <v>36</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>39</v>
@@ -1638,34 +1699,37 @@
         <v>65</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>66</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="U7" s="10" t="s">
+      <c r="V7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="5" t="s">
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1688,7 +1752,7 @@
         <v>36</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>39</v>
@@ -1709,30 +1773,33 @@
         <v>66</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P8" s="9"/>
-      <c r="Q8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8" s="10" t="s">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="U8" s="10" t="s">
+      <c r="V8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V8" s="10"/>
-      <c r="W8" s="5" t="s">
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1755,7 +1822,7 @@
         <v>36</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>39</v>
@@ -1770,38 +1837,187 @@
         <v>65</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>66</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P9" s="9"/>
-      <c r="Q9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="R9" s="10" t="s">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="S9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="U9" s="10" t="s">
+      <c r="V9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="10"/>
-      <c r="W9" s="5" t="s">
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A1:Z1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
methods for creating and deleting checklist from list are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137CD191-A863-4289-A746-105A091109DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03EE7B-9283-4DBC-AAFE-5D97C8E01220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="102">
   <si>
     <t>tc_id</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>numHeaders</t>
+  </si>
+  <si>
+    <t>numItems</t>
+  </si>
+  <si>
+    <t>headerName</t>
+  </si>
+  <si>
+    <t>saleHeader</t>
+  </si>
+  <si>
+    <t>itemType</t>
+  </si>
+  <si>
+    <t>Checklist successfully saved.</t>
+  </si>
+  <si>
+    <t>numChecklists</t>
+  </si>
+  <si>
+    <t>rowStatus</t>
   </si>
 </sst>
 </file>
@@ -476,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -512,6 +536,15 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,20 +572,14 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,25 +918,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1145,29 +1172,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
     </row>
     <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1406,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,38 +1456,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -2088,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,129 +2131,147 @@
     <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="17" width="21" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="27.42578125" style="1" customWidth="1"/>
-    <col min="20" max="25" width="21" style="1" customWidth="1"/>
-    <col min="26" max="26" width="24" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="21" width="21" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="27.42578125" style="1" customWidth="1"/>
+    <col min="24" max="27" width="21" style="1" customWidth="1"/>
+    <col min="28" max="28" width="26.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="21" style="1" customWidth="1"/>
+    <col min="30" max="30" width="24" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-    </row>
-    <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-    </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+    </row>
+    <row r="2" spans="1:30" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+    </row>
+    <row r="3" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="25" t="s">
+      <c r="J3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="25" t="s">
+      <c r="O3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="R3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="S3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="T3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="U3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="V3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="S3" s="25" t="s">
+      <c r="W3" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="X3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="Y3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="Z3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="AA3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="25" t="s">
+      <c r="AB3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="25" t="s">
+      <c r="AC3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="25" t="s">
+      <c r="AD3" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2253,42 +2298,54 @@
         <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="K4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10" t="s">
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2312,41 +2369,43 @@
       <c r="I5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="N5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="10"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Z5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="AD5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2372,41 +2431,41 @@
       <c r="I6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2432,45 +2491,45 @@
       <c r="I7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" s="10" t="s">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="R7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="5" t="s">
+      <c r="Z7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2496,47 +2555,47 @@
       <c r="I8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M8" s="10" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="R8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="Y8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="5" t="s">
+      <c r="Z8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -2562,47 +2621,47 @@
       <c r="I9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M9" s="10" t="s">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="Y9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="5" t="s">
+      <c r="Z9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -2628,51 +2687,51 @@
       <c r="I10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="10" t="s">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="R10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="T10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9" t="s">
+      <c r="U10" s="9"/>
+      <c r="V10" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9" t="s">
+      <c r="W10" s="9"/>
+      <c r="X10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="Y10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="5" t="s">
+      <c r="Z10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -2698,51 +2757,51 @@
       <c r="I11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" s="10" t="s">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="R11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="T11" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9" t="s">
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U11" s="10" t="s">
+      <c r="Y11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="5" t="s">
+      <c r="Z11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit check list is implemented
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03EE7B-9283-4DBC-AAFE-5D97C8E01220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DDEAB2-4F4F-4608-A65C-8ABC6628245F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="103">
   <si>
     <t>tc_id</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>rowStatus</t>
+  </si>
+  <si>
+    <t>checklistSearch</t>
   </si>
 </sst>
 </file>
@@ -1433,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,17 +2134,25 @@
     <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="21" width="21" style="1" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="27.42578125" style="1" customWidth="1"/>
-    <col min="24" max="27" width="21" style="1" customWidth="1"/>
-    <col min="28" max="28" width="26.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="21" style="1" customWidth="1"/>
-    <col min="30" max="30" width="24" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="21" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="23" width="21" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2170,16 +2181,12 @@
       <c r="X1" s="27"/>
       <c r="Y1" s="27"/>
       <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-    </row>
-    <row r="2" spans="1:30" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="29"/>
     </row>
-    <row r="3" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -2232,46 +2239,34 @@
         <v>57</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="U3" s="16" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="V3" s="16" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="W3" s="16" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="X3" s="16" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD3" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2322,30 +2317,24 @@
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
+      <c r="U4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="W4" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="5" t="s">
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2361,7 +2350,9 @@
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="G5" s="10" t="s">
         <v>36</v>
       </c>
@@ -2369,43 +2360,51 @@
       <c r="I5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="J5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="N5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8" t="s">
+      <c r="U5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="Z5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" s="10" t="s">
+      <c r="V5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC5" s="5" t="s">
+      <c r="Y5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="Z5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2444,28 +2443,24 @@
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10" t="s">
+      <c r="U6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB6" s="10" t="s">
+      <c r="V6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="5" t="s">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2498,38 +2493,28 @@
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>82</v>
-      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="9"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="10" t="s">
+      <c r="U7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB7" s="10" t="s">
+      <c r="V7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="5" t="s">
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2562,40 +2547,30 @@
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9" t="s">
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y8" s="10" t="s">
+      <c r="U8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB8" s="10" t="s">
+      <c r="V8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="5" t="s">
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -2628,40 +2603,30 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
-      <c r="Q9" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9" t="s">
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y9" s="10" t="s">
+      <c r="U9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB9" s="10" t="s">
+      <c r="V9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="5" t="s">
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -2694,44 +2659,30 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
-      <c r="Q10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y10" s="10" t="s">
+      <c r="U10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB10" s="10" t="s">
+      <c r="V10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="5" t="s">
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -2764,44 +2715,32 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y11" s="10" t="s">
+      <c r="U11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Z11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB11" s="10" t="s">
+      <c r="V11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AC11" s="10"/>
-      <c r="AD11" s="5" t="s">
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A1:Z1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
save checklist is not possible if there are no header and item
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DDEAB2-4F4F-4608-A65C-8ABC6628245F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250ED8C2-A82E-492E-94B0-642645092B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
   <si>
     <t>tc_id</t>
   </si>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t>checklistSearch</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>emptyCheckListMessage</t>
+  </si>
+  <si>
+    <t>The checklist cannot be empty</t>
+  </si>
+  <si>
+    <t>Headers must contain at least 1 item</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2130,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,23 +2148,23 @@
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="21" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
-    <col min="20" max="23" width="21" style="1" customWidth="1"/>
-    <col min="24" max="24" width="26.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="20" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="1" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
+    <col min="21" max="24" width="21" style="1" customWidth="1"/>
+    <col min="25" max="25" width="26.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="20" style="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2181,12 +2193,13 @@
       <c r="X1" s="27"/>
       <c r="Y1" s="27"/>
       <c r="Z1" s="27"/>
-    </row>
-    <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="27"/>
+    </row>
+    <row r="2" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="29"/>
     </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -2220,53 +2233,56 @@
       <c r="K3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="R3" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2299,7 +2315,7 @@
         <v>97</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>92</v>
@@ -2313,28 +2329,33 @@
       <c r="P4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="10"/>
+      <c r="V4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2367,44 +2388,47 @@
         <v>97</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>65</v>
       </c>
       <c r="N5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="8"/>
+      <c r="Q5" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="8"/>
+      <c r="V5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V5" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="W5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Z5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="AA5" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2430,37 +2454,52 @@
       <c r="I6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="J6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>103</v>
+      </c>
       <c r="N6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+      <c r="P6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="10"/>
+      <c r="V6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2486,35 +2525,54 @@
       <c r="I7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="9"/>
+      <c r="J7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="10"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="9"/>
+      <c r="V7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V7" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W7" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="5" t="s">
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2540,37 +2598,56 @@
       <c r="I8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9" t="s">
+      <c r="J8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="S8" s="10"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="V8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V8" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="5" t="s">
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -2605,28 +2682,29 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9" t="s">
+      <c r="S9" s="10"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="V9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V9" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W9" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="5" t="s">
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -2661,28 +2739,29 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9" t="s">
+      <c r="S10" s="10"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="V10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V10" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="5" t="s">
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -2717,30 +2796,31 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9" t="s">
+      <c r="S11" s="10"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="U11" s="10" t="s">
+      <c r="V11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V11" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="W11" s="10" t="s">
         <v>46</v>
       </c>
       <c r="X11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="5" t="s">
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:AA1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
checklist new version is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250ED8C2-A82E-492E-94B0-642645092B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18925D81-B9E4-435F-B80D-499C4A84CCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="2220" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="107">
   <si>
     <t>tc_id</t>
   </si>
@@ -913,7 +913,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,35 +2658,51 @@
         <v>9</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="G9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>69</v>
-      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="J9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S9" s="10"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9" t="s">
-        <v>72</v>
-      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
       <c r="V9" s="10" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
url is kicked out
</commit_message>
<xml_diff>
--- a/src/test/test_data/sindri.xlsx
+++ b/src/test/test_data/sindri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\contika\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809A6C9A-2BE2-4777-ADAA-80F57B5CA565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9D1037-5231-4068-928B-218D8CAABCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A605BFD-FDFD-47E6-B86E-5AAA3E9DD62F}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>